<commit_message>
Dumping code skeleton done
</commit_message>
<xml_diff>
--- a/metadata/Field List.xlsx
+++ b/metadata/Field List.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="77">
   <si>
     <t>Field name</t>
   </si>
@@ -189,36 +189,6 @@
     <t>None</t>
   </si>
   <si>
-    <t>artist_id</t>
-  </si>
-  <si>
-    <t>artist_playmeid</t>
-  </si>
-  <si>
-    <t>artist_7digitalid</t>
-  </si>
-  <si>
-    <t>artist_mbid</t>
-  </si>
-  <si>
-    <t>artist_name</t>
-  </si>
-  <si>
-    <t>artist_familiarity</t>
-  </si>
-  <si>
-    <t>artist_hotttnesss</t>
-  </si>
-  <si>
-    <t>artist_latitude</t>
-  </si>
-  <si>
-    <t>artist_location</t>
-  </si>
-  <si>
-    <t>artist_longitude</t>
-  </si>
-  <si>
     <t>track_id</t>
   </si>
   <si>
@@ -256,6 +226,30 @@
   </si>
   <si>
     <t>analysis_sample_rate</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>playmeid</t>
+  </si>
+  <si>
+    <t>digi_7id</t>
+  </si>
+  <si>
+    <t>mbid</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>familiarity</t>
+  </si>
+  <si>
+    <t>hottness</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -694,7 +688,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,7 +723,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>9</v>
@@ -749,7 +743,7 @@
     </row>
     <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
@@ -763,7 +757,7 @@
     </row>
     <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -774,7 +768,7 @@
     </row>
     <row r="5" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
@@ -790,7 +784,7 @@
     </row>
     <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
@@ -810,7 +804,7 @@
     </row>
     <row r="8" spans="1:6" ht="22.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
@@ -827,7 +821,7 @@
     </row>
     <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>9</v>
@@ -838,7 +832,7 @@
     </row>
     <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>3</v>
@@ -849,7 +843,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>3</v>
@@ -860,7 +854,7 @@
     </row>
     <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
-        <v>63</v>
+        <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>3</v>
@@ -871,7 +865,7 @@
     </row>
     <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -882,7 +876,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>65</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>3</v>
@@ -898,7 +892,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>9</v>
@@ -918,7 +912,7 @@
     </row>
     <row r="17" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
@@ -932,7 +926,7 @@
     </row>
     <row r="18" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
@@ -943,7 +937,7 @@
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
@@ -954,7 +948,7 @@
     </row>
     <row r="20" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>5</v>
@@ -970,7 +964,7 @@
     </row>
     <row r="22" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>9</v>
@@ -990,7 +984,7 @@
     </row>
     <row r="23" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -1051,7 +1045,7 @@
     </row>
     <row r="30" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>9</v>
@@ -1071,7 +1065,7 @@
     </row>
     <row r="31" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>9</v>
@@ -1088,7 +1082,7 @@
     </row>
     <row r="32" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>3</v>
@@ -1110,7 +1104,7 @@
     </row>
     <row r="34" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>3</v>
@@ -1121,7 +1115,7 @@
     </row>
     <row r="35" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>3</v>
@@ -1154,7 +1148,7 @@
     </row>
     <row r="38" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>3</v>
@@ -1187,7 +1181,7 @@
     </row>
     <row r="41" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>3</v>
@@ -1209,7 +1203,7 @@
     </row>
     <row r="43" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>5</v>
@@ -1218,9 +1212,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>3</v>
@@ -1231,7 +1225,7 @@
     </row>
     <row r="45" spans="1:6" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>3</v>
@@ -1247,7 +1241,7 @@
     </row>
     <row r="47" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>9</v>
@@ -1267,7 +1261,7 @@
     </row>
     <row r="48" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>9</v>
@@ -1284,7 +1278,7 @@
     </row>
     <row r="49" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>9</v>
@@ -1301,7 +1295,7 @@
     </row>
     <row r="50" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>9</v>

</xml_diff>